<commit_message>
finished cleaning up under the hood changes in chapter classes
</commit_message>
<xml_diff>
--- a/trackers/VORTEX 23P Tracker.xlsx
+++ b/trackers/VORTEX 23P Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\OneDrive\Desktop\Dev Projects\TM-Generator\trackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB864EE-F483-44DC-A13D-9C5E627CB8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44D6CB3-2913-4A87-8C02-8E9E4C4209ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59340" yWindow="8790" windowWidth="6405" windowHeight="4530" xr2:uid="{FC850C9D-DF54-4074-A6FC-6C313143BEB8}"/>
+    <workbookView xWindow="57480" yWindow="7755" windowWidth="29040" windowHeight="15840" xr2:uid="{FC850C9D-DF54-4074-A6FC-6C313143BEB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t xml:space="preserve">PMCS Introduction </t>
   </si>
   <si>
-    <t xml:space="preserve">PMCS </t>
-  </si>
-  <si>
     <t xml:space="preserve">M157 </t>
   </si>
   <si>
@@ -439,6 +436,9 @@
   </si>
   <si>
     <t>Troubleshooting Index</t>
+  </si>
+  <si>
+    <t>PMCS</t>
   </si>
 </sst>
 </file>
@@ -898,7 +898,7 @@
   <dimension ref="B1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -912,20 +912,20 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2"/>
@@ -933,7 +933,7 @@
     <row r="3" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="2"/>
@@ -941,7 +941,7 @@
     <row r="4" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="2"/>
@@ -949,7 +949,7 @@
     <row r="5" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="2"/>
@@ -957,7 +957,7 @@
     <row r="6" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="2"/>
@@ -972,16 +972,16 @@
     </row>
     <row r="8" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>1</v>
@@ -990,7 +990,7 @@
     </row>
     <row r="10" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>2</v>
@@ -1000,220 +1000,220 @@
     <row r="11" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B11" s="7"/>
       <c r="C11" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B19" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B27" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="5"/>
     </row>
     <row r="28" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B28" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B29" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="5"/>
     </row>
     <row r="30" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B30" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="5"/>
     </row>
     <row r="31" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B31" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" s="5"/>
     </row>
     <row r="32" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B32" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B33" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B34" s="7"/>
       <c r="C34" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>3</v>
@@ -1222,365 +1222,365 @@
     </row>
     <row r="36" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B36" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>4</v>
+        <v>133</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B37" s="7"/>
       <c r="C37" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B38" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D38" s="10"/>
     </row>
     <row r="39" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B39" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B40" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B41" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B42" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B43" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B44" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B45" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B46" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B47" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B48" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B49" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B50" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B51" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B52" s="11"/>
       <c r="C52" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D52" s="11"/>
     </row>
     <row r="53" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B53" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="D53" s="5"/>
     </row>
     <row r="54" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B54" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B55" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="D55" s="5"/>
     </row>
     <row r="56" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B56" s="7"/>
       <c r="C56" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D56" s="7"/>
     </row>
     <row r="57" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B57" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D57" s="5"/>
     </row>
     <row r="58" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B58" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D58" s="5"/>
     </row>
     <row r="59" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B59" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D59" s="5"/>
     </row>
     <row r="60" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B60" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D60" s="5"/>
     </row>
     <row r="61" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B61" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B62" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D62" s="5"/>
     </row>
     <row r="63" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B63" s="7"/>
       <c r="C63" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D63" s="7"/>
     </row>
     <row r="64" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B64" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D64" s="5"/>
     </row>
     <row r="65" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B65" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D65" s="5"/>
     </row>
     <row r="66" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B66" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D66" s="5"/>
     </row>
     <row r="67" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B67" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D67" s="5"/>
     </row>
     <row r="68" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B68" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="3"/>
     </row>
     <row r="69" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B69" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B70" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B71" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B72" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D72" s="5"/>
     </row>
     <row r="73" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B73" s="7"/>
       <c r="C73" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D73" s="7"/>
     </row>

</xml_diff>